<commit_message>
Get daily reddit data: Tue Dec 26 08:08:07 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_31.xlsx
+++ b/data/2023_12_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C446"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2471 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>18r2flx</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>got extensions for the first time! ✨</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocof268o9l8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>18r2cqf</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Nail ig page name.</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18r2cqf/nail_ig_page_name/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>18r1yq8</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Xmas/new years nails</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r1yq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>18r10zd</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Testing out a shimmery nude for New Years.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13rwhhx4uk8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>18r0lns</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Satisfying cut 🤤</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufbbz2rtpk8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>18qzzr8</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Opinions please</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyy3b4s9kk8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>18qyyhc</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Fastest/easiest way to remove gel nail polish at home?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qyyhc/fastesteasiest_way_to_remove_gel_nail_polish_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>18qyhue</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Merry Christmas!</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qyhue</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18qy0q9</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Winter ❄️ Nails</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq3gujb61k8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>18qxzh3</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Fixing gel nails that started to lift with top coat</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qxzh3/fixing_gel_nails_that_started_to_lift_with_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>18qx3k1</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>New Year’s Nails (simple mani)</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qx3k1</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>18qwxbh</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>New Year’s Nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qwxbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>18qwm3m</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Dollar tree nails 😅♥️ glue not included</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qwm3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>18qwgpa</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time ever with gel polish last night! Tips for shaping, cuticles, and cleaning up edges?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qwgpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>18qw2y0</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Logos</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qw2y0/logos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>18qvy2t</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Nail gel polish</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qvy2t/nail_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>18qvxh0</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Can you do gel polish on toenails?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qvxh0/can_you_do_gel_polish_on_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>18qvi1m</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Been natural for four months around - wanted to post before I cut !</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfosxmakdj8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>18quta8</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>First time builder gel with forms how did I do?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18quta8</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18qubc4</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>I have a cordless nail drill. I want to add bits to it, but I don’t have a way to attach them. Help.</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qubc4/i_have_a_cordless_nail_drill_i_want_to_add_bits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>18qps83</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>How do you fight the urge to do another set?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qps83/how_do_you_fight_the_urge_to_do_another_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>18qori6</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>How to remove builder gel nails?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qori6/how_to_remove_builder_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>18qm8dp</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>First time nail art! What do you think?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ocqorjt0h8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>18qu8ik</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>3-d gel</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qu8ik/3d_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>18qu4s5</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Meowy Christmas! - hand painted holiday kitties</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qu4s5</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>18qtxnk</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>❄️🌲White Christmas🌲❄️</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qtxnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>18qtt9n</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Christmas nails. 🎄❄️❤️💚</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qtt9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>18qsqmh</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>DND Cloud Castle ☁️🏰</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qsqmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>18qsleb</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Christmas to New years nails</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/753z9qwqni8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>18qsgip</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>New year disco balls!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qsgip</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18qsee7</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Christmas nail gifts</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccld9m81mi8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>18qs83b</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>OPINIONS PLEASE :)</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qs83b/opinions_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>18qs2ny</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Anyone have any recommendations for the press on nails?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qs2ny/anyone_have_any_recommendations_for_the_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>18qry1m</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Merry Christmas ♥️</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inwx49wuhi8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>18qrvkk</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Getting Nails Done For New Years Party</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qrvkk/getting_nails_done_for_new_years_party/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>18qr50c</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Happy holidays 🎄</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qr50c</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>18qr1vv</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Fresh and creamy pinks 🩷</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh9agz9m9i8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>18qr0fn</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Merry Christmas!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ed4dd269i8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>18qqsuy</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Advice on doing my own pedicures?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qqsuy/advice_on_doing_my_own_pedicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>18qqocm</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>HELP! I just did my nails for the first time and I don’t know if they look good or not. Should I keep them or not? Please rate me honestly!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocwyn2856i8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>18qq77p</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Cannot seem to get the correct nail color</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qq77p/cannot_seem_to_get_the_correct_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>18qq4zh</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Festive 🎄</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qq4zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>18qpbyb</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>My latest set. Bling bling</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efwr1qusth8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>18qp8fb</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Mickey Christmas</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qp8fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>18qp4ty</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Merry Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6xhz0qyrh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>18qon8y</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Did my Christmas nails the other day</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qon8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>18qokwa</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Beginner nails PT. 2</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erk57xktmh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>18qojxa</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>What do you think of this color scheme/style?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9t8zvhkmh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>18qoiew</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>My husbands Christmas nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qoiew</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>18qo2xc</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Christmas set 🎄</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hj3pp06ih8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>18qo1hm</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Merry Christmas!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xle4w19shh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>18qnymf</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Painted my final nails for the year</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9gcswy0hh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>18qnu1s</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Acrylic nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qnu1s/acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>18qmv1b</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Started doing nails 6 months ago</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbog392q6h8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>18qmr8t</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Christmas Press-Ons 🥰</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qmr8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>18qm1pp</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Hand-painted Christmas Press ons!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4lxk2p1zg8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>18qlvhq</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Christmas cuties I did on myself</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbh7lf6cxg8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>18qllx7</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Good quick dry top coats?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qllx7/good_quick_dry_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>18qjtux</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Some festive art, inspired by theGrayterGood ❄️❄️🎄</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qjtux</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>18qbwuj</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Custom Press Ons for the Holidays</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frbskfmejd8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>18qa227</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Thanks to everyone who helped me decide which shape to go with on my earlier post! I decided on almond—what do we think? last pic was my hand before</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qa227</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>18qkais</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>did kirby nails on myself 🩷⭐️</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qkais</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>18qk8d6</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>TIL you can use feviquik adhesive to stick nails. I did that. I love the colour and how thin the nails are and they are the perfect length. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qk8d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>18qjzaq</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Merry Christmas (nails) and happy holidays.</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16x8zx0geg8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>18qizj5</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>What are these?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xkkag2q3g8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>18qgxpt</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Getting long again!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uahz46xef8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>18qfsll</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>merry christmas to all who celebrate! here are my festive nails 🥰🎄🎅🏼</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qfsll</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>18qflc7</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>What are good, non toxic faux nail options?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18qflc7/what_are_good_non_toxic_faux_nail_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>18r12xg</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Trying OPI Reykjavik Has All The Hot Spots as a shimmery nude for New Years.</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ui1x8oqpuk8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>18r0im7</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Late to the game (story of my life this Christmas).</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3s2ra6zok8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>18r0hcj</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>After Christmas mani</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r0hcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>18r0gx1</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Merry Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xuqxb5ejok8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>18r0e8m</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>These took me an ungodly amount of time but: vintage shiny brite inspired christmas nails!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r0e8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>18r02mc</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>ILNP Mega X</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r02mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>18qz4cf</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Tried something a little different for me</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08ryhqxrbk8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>18qxmez</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Christmas Greens</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wiz3ezshxj8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>18qxfve</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Merry Christmas! 🎄✨️</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qxfve</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>18qxezf</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Merry Christmas ! 🎁</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qxezf</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>18qwv1b</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>a very sunny floridian christmas mani</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2xk2g09qj8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>18qwrby</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Quick jump to my New Year set</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3tdqeq9pj8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>18qwh1n</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>SO UPSET</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qwh1n/so_upset/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>18qwdeq</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>A Very Indie Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qwdeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>18qw77e</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Cute Color</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd3xxxr0kj8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>18qw1dr</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I didn't think it would look like this...</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qw1dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>18qvhaz</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Some warmth for the winter</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qvhaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>18qv61p</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Dupe request for Frozen Benanas by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acxby24saj8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>18qr4ms</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Olive green for a SoCal Xmas!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qr4ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>18qufvu</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Shape Help/Opinions</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qufvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>18qon9t</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>A Very ILNP Christmas</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qon9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>18quaxr</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Christmas nails (part two)</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18quaxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>18qu2kv</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Simple holiday mani ✨️</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qu2kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>18qu2ij</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Does anyone have both Dark Horse and Cinnamon</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qu2ij/does_anyone_have_both_dark_horse_and_cinnamon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>18qtkla</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Anyone know where I can find something similar to this?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ia850eojwi8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>18qtjs8</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Merry Christmas!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf7sgl5cwi8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>18qtfsu</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Xmas nails! ❤️🤍🍭 This took so long and I regret using peely base coat 🫠 but at least I’ll be able to get my NYE nails on soon!</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qtfsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>18qt6i7</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Cozy chocolate brown nails for the holidays</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qt6i7</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>18qr1ll</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Fresh and creamy pinks 🩷</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m59tqvlj9i8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>18qstr7</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Cirque colors formula seems super watery- is this nprmal or did i get duds??</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qstr7/cirque_colors_formula_seems_super_watery_is_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>18qsbx0</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Holiday red</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qsbx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>18qsagh</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Peeling issue - Need help with gel topcoat on regular nail polish</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qsagh/peeling_issue_need_help_with_gel_topcoat_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>18qs0ah</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Green for Christmas? Revolutionary.</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqr1q9yfii8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>18qrktc</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Loving nail stickers lately</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iua4d9ehei8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>18qrigg</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Hypodermic Sally Xmas color</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qrigg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>18qqs2n</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>My favourite holiday mani</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtfo5jl47i8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>18qqc2c</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Essie ballet slippers streaky?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8grmwpy2i8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>18qpopo</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>First time trying something like "nail art". It glows! 🤩</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qpopo</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>18qpml9</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Spent Christmas Eve Making Polish</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep9471jkwh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>18qpmfa</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Thank you SANTA! Need advice for this gift certificate!</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qpmfa/thank_you_santa_need_advice_for_this_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>18qpbzi</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>PSA: Polish Thinner Does Work Wonders</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qpbzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>18qowzr</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Non-Christmasy Christmas nails</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qowzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18qow4a</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>My first ever ILNP🤩 3 coats of carried away💙</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hwgd3lnph8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>18qot9h</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Matching Holiday Nails!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhrytbezoh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18qoszs</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Merry Christmas!</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qoszs</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>18qoitr</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Floral holiday mani 🌼🌲</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te64a74amh8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>18qoebb</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>LOVE this polish 😊</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/eTHMCaJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>18qodxd</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Holo Taco - Favourite Sister</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qodxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18qobrm</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Painted my nails last night in this striped cateye design! Inspired by a video I saw on Pinterest (linked) but not sure of the original creator!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/25wvudfyjh8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>18qnm0l</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Didn't quite make it to Xmas</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hcb1erondh8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>18qmthh</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>I Scream Nails; chunky glitters have not aged well</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddr0i6sb6h8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>18qmpfz</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Last Christmas i Gave you My Heart!</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qmpfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18qm8wg</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Stocking Stuffers from husband 🥰</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e96jt6sz0h8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>18qm6li</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Nails grow wonky after a certain point</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qm6li</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>18qlylj</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9nmwl87yg8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>18qllzj</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>❄️🌲White Christmas🌲❄️</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qllzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18qdao1</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>What kind of nail polish related gifts will everyone give to mother</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qdao1/what_kind_of_nail_polish_related_gifts_will/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>18qkotp</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>My nail recap from the year (some of it)</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qkotp</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>18qka8r</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Christmas ornament nails (inspo by @SuzieMoon626)</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qka8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18qjget</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Merry Christmas ladies :)</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qjget</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>18qj665</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Christmas Nails! My first time with nail art</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qj665</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18qj0kr</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Hemma free or gel for acrylate monomer allergy</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qj0kr/hemma_free_or_gel_for_acrylate_monomer_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18qirsz</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Merry Christmas! Green and gold for me this year.</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4nu2gse1g8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>18qi7e1</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Lily &amp; Fox</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qi7e1/lily_fox/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>18qhve2</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Base and Top Coat recs (UK)</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zycvmc3rf8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>18qglff</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18qglff/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>18qg1jt</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>I’m not a huge nail polish collector but my go-to CF brand Kester Black is having a “seconds” sale on stock that was damaged in a cyclone.</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqiuo4fk2f8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>18qf0xi</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>New Mani Upgrade</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qf0xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>18qeyvr</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Swamp Thing dupes?</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xulimye3ne8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>18r1wrc</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Alligator 🐊🎄🎁 Party</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r1wrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>18qyhka</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Hoping my Christmas lights mani last into the new year</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qyhka</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>18qxzu2</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Winter ❄️ Nails</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6fb8jsx0k8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>18qvj8z</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Gel polish literally peeled away for the first time ever!What happened?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/18qvj8z/gel_polish_literally_peeled_away_for_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>18qtxef</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Dark Snowflakes for a friend</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qtxef</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>18qlmrb</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>My Christmas present</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qlmrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>18qjrt4</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Just in time to post my Christmas art 🎄🎄</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qjrt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>18qjpjn</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Christmas Nails, how did I do?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/99bbec5ibg8c1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec 27 08:07:52 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_31.xlsx
+++ b/data/2023_12_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C446"/>
+  <dimension ref="A1:C592"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8015,6 +8015,2488 @@
         </is>
       </c>
     </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>18rrnlb</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>NY sets!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rrnlb</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>18ru5yw</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Gel Polish Brand</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ru5yw/gel_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>18rtyne</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Good glue for charms?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18rtyne/good_glue_for_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>18rtq8n</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>How much to charge for gel x?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18rtq8n/how_much_to_charge_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>18rtpcj</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Are these little red divots from hand washing? They crop up on my thumbnails and pointer fingers, and I don't know if cuticle oil is enough to prevent them</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqbu65fa4s8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>18rt4kh</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Kiddo did my gelx set, only her second time doing one start to finish. I think she did pretty darn good!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5irs0nyyr8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>18rt2wd</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>New Years Nails</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rt2wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>18rspyu</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Been loving airbrush nails lately 🖤❤️💚</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kj23tim2vr8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>18rs1id</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Newbie here, what would be a reasonable price for this?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psg63lyqor8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>18rrmx6</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Just tried doing my own gel mani for the first time!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as5t3hjykr8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>18rrmoz</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>First time with polygel on nail tips</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whxxt2fwkr8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>18rqord</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Press-ons and application tips for really small (adult) hands?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18rqord/pressons_and_application_tips_for_really_small/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>18rqfqd</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Post- Acrylic Stress</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18rqfqd/post_acrylic_stress/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>18rql78</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>My attempt at snowy/frosted glass nails. Not super happy with the outcome but don't hate them either. CC/tips welcome 😊</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rql78</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>18rqktj</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>NYE set 💕🎉</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09ay15labr8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>18rq3c2</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Favourite sets of 2023</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rq3c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>18rpyfb</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>My first time doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nicnurnn5r8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>18rp6m6</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Harley quinn inspired</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emj5o0ytyq8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>18roch3</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>does anyone know to prevent/fix a split nail from the side? - natural nails</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18roch3</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>18roulo</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>When I first started doing my nails and wanted to try everything lol</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pav0psywvq8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>18roq4l</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Eye nailsss by me</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18roq4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>18rokxd</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>First time using builder gel</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rokxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>18ro0jr</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>My very first time doing polygel nails</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ro0jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>18rnj3n</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwhkxalrkq8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>18rmzky</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>I’m in love! “Claire” by ILNP</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/980gat37gq8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>18rmg09</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Asking for my wife</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rmg09</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>18rmcpf</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>New Years Nails</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rmcpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>18rm3nr</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>New Year nails</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t08or2929q8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>18rm200</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Got this sparkly silvers for new years!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/986ztpqo8q8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>18rlv6l</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Husband bought me Beetles gel kit for Christmas..</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57loo0677q8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>18rll1o</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Holiday nails done by me 🎄🎁</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rll1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>18rjwsu</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Are these nails too thick or off?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rjwsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>18rjjza</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>i think this may be my fav set</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rjjza</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>18rjhw3</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Thought these were reddit worthy</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rjhw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>18rjgmb</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>I got this Nail-Care set and have no idea what most of these things are</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9c1dgknop8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>18rjdrx</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>my nail tech got me HAPPY</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abu9yalznp8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>18rirry</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>first Okay set at home</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rirry</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>18rin50</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>lacquer recommendations</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18rin50/lacquer_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>18ril3t</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>New Year’s Nails (take 2!)</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ril3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>18ri3dp</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>I have been using Seche Vite base coat and the Seche Vive top coat.</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ri3dp/i_have_been_using_seche_vite_base_coat_and_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>18rhjpz</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>My Christmas nails 🎅</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rhjpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>18r9yws</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>My art VS inspo pic! Inspo from @JennyAddem on Pinterest</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r9yws</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>18rhh5l</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>First time...</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq5n048s8p8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>18rhevf</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>This color though ❤️🎅🤍 TheGelBottle Bonfire</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rhevf</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>18rdgf0</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>nail glue for gel press-on nails?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18rdgf0/nail_glue_for_gel_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>18rafjv</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>What shape would suit my fingers?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rafjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>18r7hji</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Gel Nails Won't stay on! Help</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18r7hji/gel_nails_wont_stay_on_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>18r0nqz</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Least damage: Gel X or No Chip with Tips?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18r0nqz/least_damage_gel_x_or_no_chip_with_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>18qwil6</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Nail Art Practice Round’</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mxz33t1nj8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>18rh38k</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Nail newbie</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rh38k</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>18rgsss</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Returning to the nail tech world</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rgsss</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>18rgs0r</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My December collection</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rgs0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>18rgfdn</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Dino nails</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/midftlis0p8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>18rg5h9</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>cutie😛</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ul9sujvkyo8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>18rflld</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>cute christmas nails</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzrjmw4euo8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>18rfga3</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Went for a new shape today, a pointier tip and I am in LOVE 🥰</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rfga3</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>18rf0ss</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Any waitresses with long natural nails?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rf0ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>18qzsgi</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Art Deco Inspired</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18qzsgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>18re5qf</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>It’s giving Halloween</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18re5qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>18rdmzx</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Natural nails curling off gel</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nc9vr99ffo8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>18rd7vj</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>first time trying tortoiseshell nails!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u25ii897co8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>18rbs26</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>I’ve decided to get my certification</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe5as6i01o8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>18rbe1v</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Good?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8e7jv46uxn8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>18raywh</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>First Time doing nail art</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1i8w9jiun8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>18r9xfo</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>First time tortoise shells nails</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r9xfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>18r9vw8</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>By me, on me.</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1h8nit3pln8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>18r9ltp</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Black French tips?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zvffa58jn8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>18r9lm7</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Made myself such an unusual design yesterday, rating 1-10 pls :)</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18r9lm7/made_myself_such_an_unusual_design_yesterday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>18r9brn</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Still practicing on my own nails</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r9brn</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>18r94vy</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Rubber and/or builder gel base?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18r94vy/rubber_andor_builder_gel_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>18r90ty</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Hours poured into the 3D nails but this hand painted Santa is the one that has my heart 🎄</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r90ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>18r8yzp</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>It's a black and gold Christmas</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp73dmlhdn8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>18r7s2m</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Christmas nails (part two)</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r7s2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>18r69sm</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Abstract has been my go-to lately</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r69sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>18r5nid</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>My New Year’s Nails!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8q3nfkodm8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>18r4zjg</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>There will be New Year's designs</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31ejtfki5m8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>18r4y6f</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Bit of sparkle for the holidays 💅🥰</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20ho0pi45m8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>18r4q97</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>I absolutely enjoy this experimental (for me) gothic design done by my friend</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r4q97</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>18rvkdl</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>How do I fix my nails?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osc2140pos8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>18rvgkk</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Christmas Cocoa Jelly Nails 🤎✨</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juajvbgjns8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>18rtasu</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Looky brand</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rtasu/looky_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>18rso5a</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>PPUs</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rso5a/ppus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>18rskh5</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Full scream ahead Mooncat</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bfnt0mpjtr8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>18rrwx0</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Suggestions/Swatch Comparison Request (Pastel Collections)</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rrwx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>18rrla6</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>💅🏻Surgery Nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4cnrlzhkr8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>18rqxlc</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Pleasing (Harry Styles)</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rqxlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>18rqcxf</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Nail tech drilled acrylic off in between soaks — is that normal?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rqcxf/nail_tech_drilled_acrylic_off_in_between_soaks_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>18rq9ho</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Post-holiday detox</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rq9ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>18rq6k5</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Christmas nail stickers</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rq6k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>18rphkk</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Glass jellyfish 💜</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rphkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>18rp4aw</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>A Cristmas holos appreciation post</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rp4aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>18rp10r</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Happy Full Moon</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzsnhvcixq8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>18rowe8</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Cirque Colors Coronation (OG 2013 version)</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fx7a5xrewq8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>18rom0h</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>I’m a bit obsessed</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rom0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>18rod0q</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Nail bottle height?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rod0q/nail_bottle_height/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>18rmydx</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>When polishing your nails, Do you prefer to clean up mistakes before or after your nails dry. And what do you use (Mistakes=flooded cuticles , polish on skin ect)</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rmydx/when_polishing_your_nails_do_you_prefer_to_clean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>18rmkza</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Mani</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rmkza</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>18rm9h8</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Anybody else match their polish to the book they’re reading?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7ivb8ybaq8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>18rm478</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Moon Cat for very short thin nails?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rm478/moon_cat_for_very_short_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>18rlkr4</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>My Nails are TRASHED, help?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rlkr4/my_nails_are_trashed_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>18rkl5h</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>I started doing my own nails this past summer, it’s been a struggle but I think this is the cleanest set I’ve done so far 💅🏻</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/026del09xp8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>18rk7cu</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>dream within a dream by mooncat 🪻</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rk7cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>18rjxdw</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Love this shade for the holidays</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qil1z988sp8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>18rhubv</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>First real nail art attempt</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rhubv</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>18rjseu</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Some recent Orly manis!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rjseu</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>18rjftp</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Starlight and Sparkles Phoenix Dravite in two different lightings - OGUP (in 2023!) in a chocolate brown base</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j41vra3wnp8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>18rj0tw</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Christmas nails! Venom by ILNP for me and a candy cane manicure I did for my mom with three magnetic polishes</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rj0tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>18riavi</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>I suspect Lyn B is going to become a *problem*</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18riavi</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>18rhjry</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Christmas colors</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvx5225d9p8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>18rgrv1</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Pacifica Dupe</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rgrv1/pacifica_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>18rgobt</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Humbled</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rgobt</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>18rgewn</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Sugar cookie Christmas mani</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rgewn</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>18rfrva</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Would press ons be good for a cashier?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rfrva</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>18rfbue</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Ending 2023 in black and silver</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rfbue</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>18resy4</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Press Ons for Extra Wide Nail Beds</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18resy4/press_ons_for_extra_wide_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>18rej3j</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>My Christmas nails with China Glaze - Marry A Millionaire</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rej3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>18rednl</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I hate my nails shape they’re so.. trapzoidal (?)</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rednl</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>18recjt</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>A manicure in literally less than a minute.</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18recjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>18rdjdk</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Guitarist nails</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rdjdk/guitarist_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>18rd94r</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>When the nail art you did with your non-dominant hand turns out just as good :’)))</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rd94r</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>18rcxax</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>This in Black to Red Multichrome Flakies?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhby8k9w9o8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>18rc02g</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Ranking Every Polish Brand I Tried in 2023: The Top Ten begins!!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rc02g</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>18rbtrb</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>OPI - Alpine Snow + LA Colors - Shimmer Mist</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rbtrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>18rbouz</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>December manis — Mooncat, ILNP, BLK!</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rbouz</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>18rbdur</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>My second set of Xmas nails</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkyhdgfsxn8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>18rb3g8</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Bit late, but Christmas Mani/Dec PPU</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rb3g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>18rb1ff</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Glass Frog swatch comparison</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rb1ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>18ra652</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>First time using nail art strips! 💚</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt0rska2on8c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>18ra38m</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Loving how the dark red sets off the topper! Orly bonder, Nailberry Noirberry, INLP My Private Rainbow, Seche Vite</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a748x2u7nn8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>18ra1rq</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>You already know what this polish is, don’t you?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ra1rq</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>18r9z0u</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>ILNP Shooting Star</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xprnbcldmn8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>18r8vaf</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>🍑✨</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rzynjmicn8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>18r8465</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Some emerald green for the end of the year</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb6awat35n8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>18r70hi</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Plenty of fish in the pond 🌊</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r70hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>18r5qah</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>I did a thing!</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r5qah</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>18r4n5m</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Need suggestion gel nail polish set choice</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18r4n5m/need_suggestion_gel_nail_polish_set_choice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>18r4aqm</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Nail Stickers for the win</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r4aqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>18rv0ut</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Love my winter nails! My friend did them from her home salon! @nails by Alscena</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5e05h8fqis8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>18rqhpa</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>New Year, New Nails!</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xvmozfiar8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>18rpgqr</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Florida Nails</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t708dda1r8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>18ro82a</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Red French tips by me❤️</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ro82a</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>18rlpb8</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Jelly Nail Art</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sfxn1lv5q8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>18rjxj5</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>French but different...</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inm2iu49sp8c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>18rbtmy</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Christmas Press-On Sets</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rbtmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>18r8gss</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Questioned my sanity somewhere around the third bauble</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18r8gss</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>18r7xtx</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>⚪️🖤⚪️</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emo7678g3n8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec 28 08:08:26 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_31.xlsx
+++ b/data/2023_12_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C592"/>
+  <dimension ref="A1:C720"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10497,6 +10497,2182 @@
         </is>
       </c>
     </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>18sny6s</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Me &amp; my sister’s first ever manicure!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6b9is2ctkz8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>18snuxw</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Did these myself, not the best not the worst, but I absolutely love them.</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18snuxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>18smxg6</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Love these nails my nail tech did for me!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9g2aj2r9z8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>18smb86</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Got the IceGel Sunset powders for Christmas and couldn't decide on one colur to try 🩷🩵</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18smb86</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>18sm66e</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Unsure on shape</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sm66e</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>18slv43</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>My Christmas set :)</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3sevmo7zy8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>18slasx</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>SOS my nails are ruined</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18slasx/sos_my_nails_are_ruined/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>18sjyd3</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>First Time Frenchies</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ooxbczeahy8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>18sjhp5</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>I live in New Zealand. What products do I need for POP-OFF-PROOF PRESS ONS??</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sjhp5/i_live_in_new_zealand_what_products_do_i_need_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>18sig5c</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>I don’t know how I feel about these. Let me know what you think?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sig5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>18si9b6</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>First time ever using builder gel!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18si9b6</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>18si4k2</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>January nails ??</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18si4k2/january_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>18shizf</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Has anyone ever used nail gems? Found these at Dollar Tree tonight, curious if you've got any tips on using them.</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylyvflmzvx8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>18shgmk</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Glitter nails :)</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45wpmxdovx8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>18shdcn</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>It’s giving me old comic. Love the result.</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6e5kk0yux8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>18sfs65</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>How much should a fill cost?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sfs65/how_much_should_a_fill_cost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>18sfnm8</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Sugar rush nails</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frvy0gphhx8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>18see8a</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>First time doing any nail art</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyf8z1628x8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>18secpo</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Holiday Nails Austin, TX</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83gz8wgr7x8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>18sdyjr</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Trying a new salon.</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0dp9ger4x8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>18sdxzh</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Gel for my degree as an informatics engineer</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sdxzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>18sdryz</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Olive nails I just did!! Obsessed</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05zpmjzf3x8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>18sdro4</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Attempting to remove</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sdro4/attempting_to_remove/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>18sd7xm</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n3hlxf9zw8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>18sc2yd</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Who else is a Naruto fan?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tq8cmo3pqw8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>18sc07m</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>First time trying press/glue ons 🥰</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq9go9l4qw8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>18sbyn5</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Never get my nails done but have been growing them out for a month and decided to get a gel manicure! :)</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sbyn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>18sbrta</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Looking At Starting GelX</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sbrta</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>18sbrgz</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Sparkly Nails</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvjjn7taow8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>18sbpgb</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>it's the first time I've ever had a manicure</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gt9f9gonw8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>18sbek4</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Do nail techs usually get sued when they accidentally cut their customer?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sbek4/do_nail_techs_usually_get_sued_when_they/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>18sbcnc</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Is this set worth 145?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdpsxf25lw8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>18sag8i</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Divider only</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cvegqddew8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>18sag5i</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>😻</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ut8caficew8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>18s9peu</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Sparkly Nails - with flash and without flash</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s9peu</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>18s9jcr</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Only took me two days of sweat and tears doing my first full hand French🫠 how’d I do?😅</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqisccsh7w8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>18s92ld</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Nails by me this morning for nye</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s92ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>18s8j4u</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Girlfriend just got a Gel set and just have a few questions.</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18s8j4u/girlfriend_just_got_a_gel_set_and_just_have_a_few/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>18s86xc</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Love these ombré nails</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s86xc</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>18s85xo</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>almost forgot to post my holiday nails</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s85xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>18s84qf</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Flower power 🌸</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7npxb6xwv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>18s8214</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>New year new nails right?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41r27f3dwv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>18s7zaf</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Got them done 🤍</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mhjlelsvv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>18s7lii</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Not sure how I feel about out this French.</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s7lii</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>18s7iz1</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Growing natural nails 🌿💅🏼🌸</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s7iz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>18s7gm7</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Gel polish recommendations</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18s7gm7/gel_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>18s7bag</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>they look bad. can i fix or should i have them fix it?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s7bag</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>18s77rx</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>The best nail set I’ve ever had</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s77rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>18s6t1f</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Regular polish 💅🏼</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79vqcw64nv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>18s6hre</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>New set(ish).</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s6hre</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>18s5ym7</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Freshly shaped nails are the best feeling</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9ib6inqgv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>18s5iuy</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Im brand new to doing nails and I did these myself! Any thoughts or tips?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s5iuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>18s5cm1</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Solid gel glue for tips</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18s5cm1/solid_gel_glue_for_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>18s56vs</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>gorgeous reflective polisj</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/igk5pr32bv8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>18s3mvf</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>any tips on cleaning the sides of nail “perfectly?”</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yzyammwyu8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>18s4qc3</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Fixed my nails!</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s4qc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>18s2qjb</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Recommendation for a peachy pearl nail powder?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18s2qjb/recommendation_for_a_peachy_pearl_nail_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>18s44y3</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Bonus pic of *the process*</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s44y3</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>18s43k8</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Removing Acrylics</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18s43k8/removing_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>18s3w4i</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Icy</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ki92red11v8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>18s3v0z</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Tb to my favorite nails I've ever done on myself.</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s3v0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>18s3t0i</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>I’ve always liked having long nails except when typing 🥲</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s3t0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>18s2xad</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>I'm really happy, from my jobs 2 years after I started.</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s2xad</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>18s2q6e</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Good starter acrylic kits?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18s2q6e/good_starter_acrylic_kits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>18s2h2d</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Gels</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s2h2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>18s0vpn</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Brand new to press on nails!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18s0vpn/brand_new_to_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>18rzskm</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Thoughts on design?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g9tj2ai1u8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>18rzgvy</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Velvet style</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lz6ioe2yt8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>18rz0xp</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>My first almond shape 😊</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rz0xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>18rydfb</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Sparkly nails ✨✨</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rydfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>18rxvar</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Thoughts on my gel-x sets?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rxvar</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>18rwpgh</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Were these done wrong?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18rwpgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>18rw26z</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Do they look ok?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gn41o79bus8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>18rvo67</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>first time using builder gel in a bottle</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aeu6gpesps8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>18sojyq</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Where to start?!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18sojyq/where_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>18smrsb</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Polish recs like this salon manicure ?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81ytatf38z8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>18slbyz</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Recommend me a top coat</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18slbyz/recommend_me_a_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>18ska3k</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Lumen Prototype</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ska3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>18sjw1k</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Best French Tip Base Recommendations</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi2p0owpgy8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>18sjrm1</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>OPI Less is Norse.</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sjrm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>18sine3</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>nail polish shelf</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ydcpg2s5y8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>18si1oe</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Last Gel Mani - Got Myself an Allergy</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukqp5sim0y8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>18si188</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>New mani for what's left of the week 💅🏻 Almost there searching this entire collection! - Kiko Milano Perfect Gel shade #110</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18si188</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>18shoa1</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>First Ombre</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18shoa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>18shnds</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Liberace called...</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18shnds</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>18sgrgx</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Kermit me to speak</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sgrgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>18sgd1x</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Tragedy struck, and then my dragon found his rider!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sgd1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>18sezfx</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Lavender Chill ❄️</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sezfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>18sdoxc</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>My nails for NYE ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtb2ucls2x8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>18sdgra</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Not Feeling the Holiday Vibes…</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sdgra</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>18sdehb</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Post Christmas Mani</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zndi509n0x8c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>18sd136</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Velvet hack set up + result</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qf3kkw6txw8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>18sc2nu</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>some of my December nails</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sc2nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>18sc19o</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Mooncat - Loch Ness</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sc19o</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>18sc0gl</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Mooncat Monster Under Your Head</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sc0gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>18s9uv4</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Glass Jellyfish</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s9uv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>18s9kve</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>First try with the Cirque tortoise shell set 🤎🧡</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nyyg13ut7w8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>18s9fe0</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A BKL Classic </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/83y6wwmm6w8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>18s8j6o</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Obsessed with my holiday nails, magnetics truly make everything look magical, even when you're stuck with shorties!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s8j6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>18s86e0</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Is the gap between my cuticle and my polish too big?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s86e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>18s7yzs</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>My favourite shade ever</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lcwggwqvv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>18s7c8d</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>ILNP Legacy v HT Amber Apathy (dupes?)</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s7c8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>18s6r6j</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Dupe Alert: Once upon a dream and Cosmos the space dog</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s6r6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>18s44bd</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>My favourite polishes this year</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s44bd</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>18s3xci</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Swipe for a peek behind the curtain</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s3xci</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>18s3oww</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>This ILNP chrome is wild! I had someone ask me if it was a dip manicure.</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc8wlsgdzu8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>18s2rh1</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Ranking Every Polish Brand I Tried in 2023: The FINALE!!!</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s2rh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>18s2pff</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>I have a type?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s2pff</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>18s1o49</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>The perfect winter glow</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s1o49</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>18s1gl9</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decide to try The Wizard Topcoat on its own. </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/irj93vm1hu8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>18s11ei</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>I love icy winter blues ❄</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s11ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>18rxawe</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Baby I can see your Halo</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hkss6yd99t8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>18rvrmv</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Fave YouTube (Shorts) channels?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18rvrmv/fave_youtube_shorts_channels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>18soi2k</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>help :))))</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18soi2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>18slgmw</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>random press ons i found in my collection</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9yqk45dvy8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>18sjlo7</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Japanese manicure</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8rfrp5k2ey8c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>18shz0u</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Lil Winter Sweater Set</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18shz0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>18sh2hx</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Krampus nails for the season</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/RzbBSD4</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>18sev5b</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>New nails I do today</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvpqhmalbx8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>18seasn</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>So fresh and so clean clean</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xeczp7c7x8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>18sdqwj</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Five hours of practice, flowers flowers</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/501eavm33x8c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>18sdn9g</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>⛓️chrome for nye⛓️ done by me🩶</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sdn9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>18sclwe</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Dollars what we all want 🥵 design for my client 🥰</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3n9qsnxmuw8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>18s95ls</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>December nails</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v778s9vk4w8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>18s77wx</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>I think I found my signature look! Went for a subtle black and blue-grey ombre.</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18s77wx</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>18s6fb0</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Getting a fresh look today, but had to show these off one last time!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xohk5hqakv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>18s3wm1</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Icy</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rdh4fm51v8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>18ryihp</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Green jelly over magnetic cat eye</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if0vl03bnt8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec 29 08:07:52 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_31.xlsx
+++ b/data/2023_12_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C720"/>
+  <dimension ref="A1:C894"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12673,6 +12673,2964 @@
         </is>
       </c>
     </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>18th8w4</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>last set and current set :)</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18th8w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>18tgqn9</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Sassy Cats Sugarcoat Everything - A subtle, glowy win.</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tgqn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>18tgjw7</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>If your shellac/gel started lifting after a week, would you go back to get it redone?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tgjw7/if_your_shellacgel_started_lifting_after_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>18tg7qg</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I know big gems aren’t for everyone, but, it is New Years.</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tg7qg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>18td62y</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Are these as bad as I think they are?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18td62y</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>18tb521</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Winter/New Year’s nails ✨❄️</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tb521</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>18ta2v2</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>How to fix press ons too curved/tight on flatter natural nails</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ta2v2/how_to_fix_press_ons_too_curvedtight_on_flatter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>18t6n4n</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Total Newbie, need advice on nail shape and how to take good photos of hands because ring pictures</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18t6n4n/total_newbie_need_advice_on_nail_shape_and_how_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>18t659k</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Dip nails and longevity?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t659k</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>18t4n3v</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>New Year’s Nails</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mt8u5ytmp39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>18t3wx1</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>back again with more thermal reactive colors for new years!! 💜🥳✨🩷</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t3wx1</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>18tg2tl</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>UV Gel Refill Pricing</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tg2tl/uv_gel_refill_pricing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>18tf3qm</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Mom's newest mani! New years edition!</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tf3qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>18tf12u</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>my year in nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tf12u</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>18te5s8</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>New set with gel liner polish I got for Christmas!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2no4t5yu59c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>18tdfze</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Tell me it's not as bad as I think it is 😭</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tdfze</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>18tddkp</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Do you wait for your nails to chip to trim them?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tddkp/do_you_wait_for_your_nails_to_chip_to_trim_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>18td5sc</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Hands are wierd:)</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrnd8c31m59c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>18td4f8</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Semi-Cured gel strips?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18td4f8/semicured_gel_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>18td386</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>My natural nails right now, what should I get at my manicure done tomorrow?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2xo8oyel59c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>18tculu</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bit of sparkle </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tr2ppyu9j59c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>18tcrq8</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Blank slate for the new year</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/we5jrlyni59c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>18tcmzm</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>New Year’s Nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tcmzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>18tbyyk</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Red n’ spicy nails 🔥</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztot9tkqb59c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>18tbfhf</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>💖 In love</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tbfhf/in_love/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>18taxbv</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>I was going for a Snow Globe look ☃️ (please excuse the shakey hands 🫠)</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5l12xtt259c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>18tal6t</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Baby Blue Stilettos</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve9a2jlxz49c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>18ta9ep</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>I'm not so much a fan of encapsulation, I think my work on it doesn't look that good.</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/303x9ooyw49c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>18ta9b6</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velvet Nails for New Years! </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yq8upe24x49c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>18ta6ql</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Magnetic nails</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ta6ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>18t9dz5</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>I tried dip powder for the first time on myself pls help 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t9dz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>18t91p4</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>new mani. wearing a sheer pearlescent shade. 🤭💎✨</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28z8xgh9n49c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>18t8ynm</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Removed the acrylics and did gel on my natural nails + cute stickers</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t8ynm</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>18t8cw2</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Tried some new full coverage tips from Sally’s</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmwvgfirh49c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>18t8b6b</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>In love with this new nail salon I'm going to</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st6fzw6dh49c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>18t85or</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>I hope this didn't happen to anyone on this sub:</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18t85or/i_hope_this_didnt_happen_to_anyone_on_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>18t82hn</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>my first time doing nail art on myself! and my fifth set in general i’ve done. GEL x.</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xbtku7ff49c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>18t6biu</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Grabbed two random colors from my box</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05ynaqf3249c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>18t1oox</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Damage from acrylics!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/li0444f4339c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>18t5qz9</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>What shape best fits my nail length?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t5qz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>18t5ddi</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Surprise cat eye</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0svcp9m0v39c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>18t54rp</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Tried a new color</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pd04ur9t39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>18t4pc6</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Blue chrome featuring morphe eye shadow 🤣</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boio5003q39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>18t4k9y</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Nail shape</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oco1ajy1p39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>18t47hx</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Yes or no?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eohs0wpgm39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>18t3ufh</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>I hope everyone had a good Christmas🎅❤️</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vs7lpspoj39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>18t33xa</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>🤍🩶 ILNP Snow Angel and Sled Day ❄️🛷 Bringing a little winter to California</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t33xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>18t325q</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Second attempt at nail stickers💫</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/escutkhmd39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>18t2v9s</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Swirly chrome French</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4umy95u6c39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>18t2q9u</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Amazon Dip Powder</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18t2q9u/amazon_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>18t2fkk</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>A year in review (minus a few sets I didn’t save)</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t2fkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>18t2a97</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>I didn’t get the puppy I wanted for Christmas but I got these and I’m not mad about it 🥰🥰🥰🥰🥰🥰</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t2a97</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>18t22c5</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>I never get my nails done but have been browsing this sub and really wanted to try tortoiseshell nails.. I got them today and I can’t tell if I like them or they are super wonky and weird?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t22c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>18t1ruw</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Winter blue❄️</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t1ruw</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>18t1jah</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>I will stalk my nail tech if she ever leaves me</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8od6lvp0239c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>18szxnl</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>help??? first acrylics, wtf went wrong</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18szxnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>18t0uzo</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Some press ons from a Local Bubble tea shop</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmh0k0vzw29c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>18t0btw</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Rose gold winter nails</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s17559z1t29c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>18szqbc</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>I always go back to red! ✨</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28ebupjpo29c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>18szicu</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>how often can i redo my nail sets?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18szicu/how_often_can_i_redo_my_nail_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>18szgqs</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>NYE Nails</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18szgqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>18sz8g7</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Hearths &lt;3 by me</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sz8g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>18svojz</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Nail drill</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omh0kn86u19c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>18svmbr</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>What do I use it for?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqdg7wbnt19c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>18sr48s</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>How do you put oil on nailbeds?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sr48s/how_do_you_put_oil_on_nailbeds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>18sz20j</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>nail care advice?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sz20j</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>18slylj</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Which nail shape?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18slylj</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>18sirwu</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Anyone tried HolyGels?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cklhjwt6y8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>18siiud</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Multipacks of acrylic press ons, and running out of your sizes..</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18siiud/multipacks_of_acrylic_press_ons_and_running_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>18syfkb</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Birthday/NYE bling nails</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18syfkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>18s88fg</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>December nails</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nk0edmvnxv8c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>18sybqz</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Holiday Szn</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyl8m4yce29c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>18sy04j</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Yay or nay ? 🤭</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sy04j</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>18sxxby</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>What am I doing wrong? My French tips are chipping off</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sxxby</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>18sxt3g</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Remove residue from decorative decals..</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sxt3g/remove_residue_from_decorative_decals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>18sxsju</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Looking for some good supplies, any advice is appreciated!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sxsju/looking_for_some_good_supplies_any_advice_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>18sxkdm</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>New to nails please help</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sxkdm/new_to_nails_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>18sxi49</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Ditched Gel forever</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l88h95b829c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>18sx5or</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sx5or/beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>18swzjh</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>New Year’s nails of my dreams 🤩</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18swzjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>18sw8au</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>After Christmas/New Year’s/Winter Mani</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sw8au</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>18sw7ow</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>My favorite I've had all year</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcqr6z39y19c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>18svo8c</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>2nd time using acrylic, how did I do?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18svo8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>18svabl</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>my first attempt at a mani</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18svabl</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>18suq49</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>My snowman and me</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18suq49</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>18su9j8</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>I love them, whatever they say</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g36i8lbei19c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>18su70a</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Tried chrome for New Year’s and I love it 🤍</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fxr0h0sh19c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>18su2zm</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Deep Blue metallic Stiletto nails</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18su2zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>18sty8k</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>A husband on a mission - last night's manicure</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sty8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>18stsl5</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Couldn't decide on one colour🩵🩷</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18stsl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>18stfed</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>How to make the glitter French tips less chunky?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18stfed</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>18stbut</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55n743ot919c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>18sspok</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Anybody know some good nail salons in Bakersfield, Ca ?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sspok/anybody_know_some_good_nail_salons_in_bakersfield/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>18sskg0</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Skittles nails with la colors color craze gel - pink sugar as a topper</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ve859a7219c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>18sr8gw</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>How do they look?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sr8gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>18sqn24</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>My sister's friend did thus, and I'm in love 🥰</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sqn24</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>18sqb19</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>First time Gel Builder - any tips?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sqb19/first_time_gel_builder_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>18sq60f</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Christmas gift from my wife</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sq60f</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>18sq605</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Does glitter polish stain nails ?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18sq605/does_glitter_polish_stain_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>18spvem</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Cue Babylon zoo ‘spaceman’</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5598j70h709c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>18thon1</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Thoughts on these cheap cheap pressons?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tpkwbgxu69c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>18tf6ml</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>I don't give ILNP toppers the credit they deserve</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tf6ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>18tepi8</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Be honest 😭</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tepi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>18t5qdp</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>If you’re thinking you need Shooting Star, you’re right</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4v24n5vpx39c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>18tdr3i</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>🎄 (Belated) Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s9cbsp8cr59c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>18tdlje</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Press Ons Gave Me C Curve</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tdlje/press_ons_gave_me_c_curve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>18tdiym</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>🎆 My NYE Nails! 🎆</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n7xa6rmap59c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>18td1x2</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Cirque Colors Mobius (velvet style)</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/whkv2wo2l59c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>18tcnkn</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>This Color's Making Waves</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mk8xnlmnh59c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>18tcfz9</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Black Holo Wish and Rainbow Snow</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tcfz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>18tcdut</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>NYE Disco Ball Nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8109ckbbf59c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>18tc7a9</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Going ethereal for the new year.</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/jUWryNe.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>18tbfyl</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Reels?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tbfyl/reels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>18tbftd</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tbftd</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>18tba91</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Obsessed 😭 Mooncat From the Ashes</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dd618fwv559c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>18tba0n</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>First time acrylic set</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tba0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>18taok0</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>6 Nail Polishes that surprised me (in a good way) -2023</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18taok0</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>18tanzr</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Glass Jellyfish and First PPU Haul!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tanzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>18t8xwq</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>First polish worn from my DRK Nails Nail Polish Lab from August PPU</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t8xwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>18t8qn9</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>🩸 ‘Carrie’ 🩸 by ILNP</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlmprp5rk49c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>18t8mj5</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>An old fave this week</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsu1v8iwj49c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>18t8l0v</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Tomb of Wrestlers by Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t8l0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>18t8jbw</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Cock a doodle doom</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t8jbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>18t8atm</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>To the people who found that ORLY Bonder base coat shredded their nails</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18t8atm/to_the_people_who_found_that_orly_bonder_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>18t82cd</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>What a stunner!</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t82cd</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>18t7w7w</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Sugarcoat Everything</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t7w7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>18t6ke7</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Never underestimate an essie shimmer 😭</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu66ptpy349c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>18t5s2d</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>The One Where I Got More Nail Mail...</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t5s2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>18t5lnf</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Neon Black</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaeoccvpw39c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>18t4vh6</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>ILNP Ava</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t4vh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>18t4p6v</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>ILNP On the Rocks</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af766pi2q39c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>18t3hz6</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>ILNP Rosewater</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t3hz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>18t3eb6</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Kraken’s Wrath 🐙💚</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nzkg88bzf39c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>18t3dsi</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>ILNP - Dream Girl 🌸</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t3dsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>18t3ctn</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Soft Overcast Gradient</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t3ctn</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>18t32yx</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>🤍🩶 ILNP Snow Angel &amp; Sled Day ❄️🛷 Bringing a little winter to California</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t32yx</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>18t2qh7</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Removing gel polish</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18t2qh7/removing_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>18t2iaj</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>🐦 🌈</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t2iaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>18t2g03</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Me: “I’m a minimalist, I think” also me: “this is a palate cleanser, right?”</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t2g03</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>18t26w7</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Handsome Mount</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty3siemx639c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>18t247m</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>The aftermath of holiday cooking.</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t247m</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>18t1vq3</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Couple magnetic comparisons - Paradox &amp; That Seems Ominous</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t1vq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>18t1l1t</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>my first attempt at nail designs</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t1l1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>18t1ev3</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>I keep walking around to different lighting trying to catch my favorite shift. This is it</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/40n1aia2139c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>18t0xnr</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>My first boutique polish!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36o1vtpix29c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>18t0r1g</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Question about nail vinyls</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18t0r1g/question_about_nail_vinyls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>18t05fz</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Christmas Lights 🎄</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t05fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>18szohk</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>IlNP first timer 🤩</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tiw1t03co29c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>18szdkf</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Treatment for peeling nails and dry cuticles?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18szdkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>18sz850</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Nail nail mani pt 1!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sz850</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>18syn6t</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Hidden Shimmer Polish Recs</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18syn6t/hidden_shimmer_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>18syetl</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Glass jellyfish!</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyi0o1a0f29c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>18syab8</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Macchiato Cloud under a street light</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/euzhxhg2e29c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>18sy2ek</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>degeneration!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sy2ek</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>18sy1fn</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Mid-Holiday Week Palate Cleanser</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sy1fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>18sxe5f</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Mint Money</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sxe5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>18sws9t</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>After years of bad dermatillomania my nail grows oddly, any tips for filing/proruct to help get it to a nice shape?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18sws9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>18swho3</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My first time: Gel extensions</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18swho3</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>18svr3g</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>{Gifted} Super shimmery 😍</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgojs6oru19c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>18svqhk</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>best qdtc for glitter polish?</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18svqhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>18stn8c</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>No snow outside, trying for snowy nails!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mj30z0rc19c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>18srgy5</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Does anyone know a dupe for this? (Major Dijit Chameleon Nail Polish in “Sweet”)</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18srgy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>18spx5a</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Decided it was time to swatch my collection</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9po4rzt1809c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>18soz6f</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Circuit board nails -&gt; steampunk circuit board</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18soz6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>18tgaoj</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>I know big gems aren’t popular on Reddit, but, it is New Years</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tgaoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>18tf4d3</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Mom's newest mani! New years edition!</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tf4d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>18tczf8</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Rate my lil Santa hehe</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yddelahk59c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>18tctq0</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Sparkly New Year Nails</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nu8tc1b2j59c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>18tb326</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Self made: I wanted a little snow globe look ☃️ (please excuse my shakey hands lol)</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1sckjad7459c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>18ta87f</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Every day I take a little bit less time, how can I improve my times? I did all these designs in 7 hours. Is it just practice?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ta87f</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>18t8gd8</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>First design I ever did</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18t8gd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>18t6yy6</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Done in Canada Ontario ChiChi nails 💅 I absolutely love them</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnmwktj0749c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>18t6xj6</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Find the butterflies😍😍 beautiful design for my client today 🎀</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/riemwitp649c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>18t04yp</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49n5mlrpr29c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec 30 08:07:25 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_31.xlsx
+++ b/data/2023_12_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C894"/>
+  <dimension ref="A1:C1076"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15631,6 +15631,3100 @@
         </is>
       </c>
     </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>18uag5x</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>What do we think about this colour on me?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dyivaxb1e9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>18u9hea</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Design in procreate VS reality</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u9hea</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>18u8tod</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>When you’re sad to let a set go</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s47du2ayjd9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>18u8g9o</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Happy New Year nails!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u8g9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>18u80cz</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>green beetle nails</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbn5yixtbd9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>18u7usw</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Thoughts on these ones? Done by me</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u7usw</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>18u7ofs</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>First natural nail manicure</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rroeln9k8d9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>18u7l9e</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>How to cure glitter dip or chrome powder?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u7l9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>18u77m0</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Did this beautiful set on a client yesterday :)</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u77m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>18u764k</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>My 5th attempt painting nails!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u764k</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>18u5uae</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Why do my almond nails look like this from the side?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u5uae</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>18tzeyp</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>My best friend does my nails for me and here’s some of the styles she’s done for me this year!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tzeyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>18tye27</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>what I got (@nailsbysandyyy) vs the inspiration (@evelinail_art)</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tye27</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>18ty3dh</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Help please 🙏</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ty3dh</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>18u5vyb</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>2023 of nails</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u5vyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>18u5ufo</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Might be a stupid question?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18u5ufo/might_be_a_stupid_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>18u5hwi</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>New Year’s Eve nails</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mq86issnc9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>18u4jaq</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Looking for dupe: Sally Hansen Strengthening Nail Polish Remover</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbdv0r26fc9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>18u4ehy</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>New Year’s Nails</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u4ehy</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>18u48jq</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Did these press ons cause I’m on a budget 😝</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cs756ahcc9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>18u380c</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>I HAVE NO IDEA ON HOW TO DO NAILS</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u380c</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>18u1tur</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Holiday nails!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u1tur</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>18u1r9t</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>In my disco ball 🪩 fish scale 🐠 alien 👽 robot 🤖 tin man 🪙glitter ✨ rainbow 🌈 era 😉</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u1r9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>18u1noj</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Got a new set 💕</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u1noj</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>18tw3zr</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>obsessed with these!!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrr5h6aija9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>18tv26y</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>First x gel done on me !</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cbe8xn3fba9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>18u0sev</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u0sev</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>18u0saa</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>These nails have a chokehold on me</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u0saa</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>18u0qqm</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>My nails when they were freshly done!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u0qqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>18u0ow6</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>I LOVE them. Clean nails for the New Year</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u0ow6</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>18u0eug</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Only possible to do this with acrylic? Huh?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qluoidvgb9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>18tzwu9</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>New color. 💙or🚫.</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn7i196wcb9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>18tztku</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Making a case for red chrome 💅🏽</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tztku</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>18tzrld</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>First time doing my own french manicure! They’re not perfect but I really like them 😊 what do y’all think? This is with full cover gel tips and gel polish</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tzrld</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>18tznza</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Cat eye not cat eye-ing ??</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6h77e00bb9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>18tz8ij</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>First (and probably last) time water marbling my nails!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tz8ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>18tz85q</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Naked once again ( ´△｀)</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tz85q</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>18tz7i4</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>New set, middle finger glows in the dark too ;)</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tz7i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>18tz18i</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>New year nails! 💚</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ocupi966b9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>18tys0q</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Is this normal for gel polish?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tys0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>18tyn9f</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Naked nails</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5p7843x83b9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>18tyhx9</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>ILNP “After Hours” Magnetic Polish</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tyhx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>18tyfnp</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Is it normal for dip to be over the tip like this?</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tyfnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>18tyb43</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>2024 New Years</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tyb43</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>18ty0ku</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>i got a gift certificate to a new salon in my area</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ty0ku</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>18txy2f</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>OPI Polish</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18txy2f/opi_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>18txjx5</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Natural Nails/Light Blue Cateye (after biting my nails for my entire life)</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfif0c9mua9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>18twtdz</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>I’m never giving up my nails lady even with HCOL and all!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwvtgcnwoa9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>18twngp</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>went full glitter for new years 🎊</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzl5ivcmna9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>18twn6d</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Another 2023 year in nails!</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18twn6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>18twjkt</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>I did someone else’s nails for the first time, this is how they came out</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18twjkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>18tvuqz</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>How to remove press ons</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tvuqz/how_to_remove_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>18tvsgl</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>New Years Nails</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74u3nam3ha9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>18tvcwz</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>My 2023 nails hopping on the bandwagon)</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tvcwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>18tv7uy</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Loving this color</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8e2cqrboca9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>18tv2no</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>It’s off center😭</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8j6f95jba9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>18tv057</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Getting ready for 2024, what you think?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tv057</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>18tu6ja</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>I have regrets</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr8ax8np4a9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>18tttjq</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Nail bed growth before and after doing my own nails</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tttjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>18ttsy8</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>can i put top coat on top of a gel manicure?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ttsy8/can_i_put_top_coat_on_top_of_a_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>18tts5m</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>New DND polish seems thick??</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tts5m/new_dnd_polish_seems_thick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>18tteqa</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Don’t know how to feel about ILNP Deep Space magnetic polish.</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1uy4canpy99c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>18ttegg</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>2023 Nail Recap (364 Days since my first gel set on myself)</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ttegg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>18tta3v</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Kiara Sky Diamondfx acrylic power</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tta3v/kiara_sky_diamondfx_acrylic_power/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>18tt3no</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>My new years nails!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tt3no</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>18tsyru</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>These are the worst nails ever</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/espasrodv99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>18tssjv</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Can I use builder gel to apply Dollar Store nails?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tssjv/can_i_use_builder_gel_to_apply_dollar_store_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>18tsm3m</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>No plumbing pedicure basin</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck1txc3qs99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>18tsjwn</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>I've been doing nail swatches for 2 hours and I'm losing it</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tsjwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>18ts4j9</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>New years nails</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcmy5x4yo99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>18trz7a</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Chocolatey Gold Cats Eye - Anyone else immediately get their Christmas nails off to try out Christmas gifts?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxy5k2trn99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>18tr5c9</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Overcuring nail polish?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tr5c9/overcuring_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>18tqg4e</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Tell me I'm wrong.</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tqg4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>18to7sw</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Glitter bomb w/eczema 😑</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ghzivvut89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>18tjpyf</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Nude shimmer nails</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tjpyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>18trl7p</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9oy76nrk99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>18trikf</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Something simple for the holidays! 🎅❄️</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18trikf</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>18trhya</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>did a little diy for New Years, little crooked sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o214nl24k99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>18treu3</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Late but Xmas nails (me &amp; my little)</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phvxfqzej99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>18trcij</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>First time in a while</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86zlriywi99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>18trb8g</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Should I use the nail glue that needs to be cured or just nail glue?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18trb8g/should_i_use_the_nail_glue_that_needs_to_be_cured/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>18tpyyq</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Not a pro but I’m proud of myself</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tpyyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>18tpy8m</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Forgot to show yall my Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tpy8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>18tpusg</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>My Bf dropped a hint that he plans to propose for my birthday in a few weeks. Color/design ideas for engagement pics? Not sure if this is the right place to post this, sorry if it’s not!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tpusg/my_bf_dropped_a_hint_that_he_plans_to_propose_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>18tpsi5</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Probably my favorite set I’ve done!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tpsi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>18tpq0g</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Love these</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxrgnz68699c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>18tpo8v</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>End of year nails</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4yjm69v599c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>18tpmqi</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Simple gels</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tpmqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>18tpajj</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Hi! New here! Appreciation post for my nail tech</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2ycdclr299c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>18tp6bs</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>NYE nails</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inqf5ljt199c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>18toqqu</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>My 2023’s manicures 💅 What’s your favourites? 💖</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18toqqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>18tohjb</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Can I get a tip on my broken nail?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cceexv5w89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>18tnws7</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Why do I hate them 😭</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tnws7</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>18tnfby</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>New set for the last working day of the year</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il3ie7qxm89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>18tn9jz</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Beginner practice💚</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tn9jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>18tn0n6</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Since you like it, maybe another cow?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s23wix01j89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>18tmxqt</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>my new year nails✨</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tmxqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>18tmuy6</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>My first ever set!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5dn00cjh89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>18tmr25</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>New colour for me</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tmr25</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>18tmh8x</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Second hand nail curing lamp?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18tmh8x/second_hand_nail_curing_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>18u9tmx</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>New Year Nails</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/le8r6y0cud9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>18u9k3g</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>I love when family lets you practice. I'm so happy to have so much support from them (:</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmwb6rohrd9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>18u8m2q</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>New Years mani!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u8m2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>18u8izy</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Jet Setter more purple than pink</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u8izy</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>18u8h9t</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Jelly is officially my favorite finish!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihii5gsigd9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>18u7w6j</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>I've been feeling very 2011 Tumblr vibes lately, and I'm gonna lean into it</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3zddxroad9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>18u551u</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Dazzle Dry System Question</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18u551u/dazzle_dry_system_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>18u6g8h</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>New years nails ft HOTD ring</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u6g8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>18u6ewp</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Winter design experiment!</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u6ewp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>18u6ajr</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Are ANY Nail Polishes Acrylate free??</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18u6ajr/are_any_nail_polishes_acrylate_free/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>18u5l76</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Tried blooming gel for the first time 💓</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4p36dtanoc9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>18u4xng</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Ghost or Grandma</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18u4xng/bees_knees_ghost_or_grandma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>18u4qa8</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>GelMoment sparkles for my mom and me</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1pnqrlwgc9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>18u3tp1</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I hopped on the Holiday Swatching bandwagon....</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90jcc80t8c9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>18u2qpd</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>first time using magnetic polish! i can’t stop staring 😍</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rv5ckmemzb9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>18u20yt</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>New Year Nails! First time going dark.</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrxsm0zmtb9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>18u1mvv</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Budget cuticle oil recommendations?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18u1mvv/budget_cuticle_oil_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>18u183h</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>how tf do you easily remove glitter polishes? specifically Holo Taco Naughty List</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18u183h/how_tf_do_you_easily_remove_glitter_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>18tyyt7</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Does anyone know what this is?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tyyt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>18tzw3h</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Ready for a vampy new year... 🦇💅</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tzw3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>18tzu1o</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Moody NYE GelX set 🥂</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tzu1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>18tzrgt</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>My Year in Polish: 2023</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tzrgt/my_year_in_polish_2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>18tzm8k</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Winter Look</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tzm8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>18tz374</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Nail Art after 20 years of nail biting</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tz374</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>18txsq4</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>I love sparkles</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18txsq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>18txr15</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Daryl’s Hunt from LBOH nov 23’</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18txr15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>18txqlc</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>What do you do when you're quarantined over Christmas? Swatch your entire nail polish collection!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18txqlc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>18txmrc</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>I understand the hype now. Fairy Dust is magical.</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18txmrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>18txeog</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Ella + Mila After Party 💕💿</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18txeog</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>18txemw</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Blue Cateye</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pg21smbgta9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>18tx7r8</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>I found this at the Dollar Tree while I was out and about today and was wondering if anyone else in the subreddit has tried this brand before</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tx7r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>18tx79p</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>The only reason I purchased Orly Bonder</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1214y7jura9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>18tw154</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>My 2023 compendium of polish: eighty-eight annotated manicures</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tw154</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>18tvur5</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>NYE ❄️</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sa0g1g6lha9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>18tvntm</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>OPI - OPI ♡ DTLA</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tvntm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>18tv9ie</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Such a pretty color</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vshogzr0da9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>18tuxox</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>I figured it was only fair to go crazy for my last mani of the year!</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lorv9hgaa9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>18tuozg</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm4lssrl8a9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>18tu1nl</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>How do you guys go about letting a broken nail grow out?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tu1nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>18ttzsn</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Appreciation post</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdpe58993a9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>18ttzc3</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Some of the polish I got for the Holodays</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ttzc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>18ttxow</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>[Builder gel] + regular polish mani</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ttxow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>18ttmly</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>NYE sparkle</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ksya64wf0a9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>18ttago</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Hunting down a polish from the 1980s</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ttago/hunting_down_a_polish_from_the_1980s/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>18tt5g1</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Glitterrific</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wx1tq1ssw99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>18tt3cs</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Easiest ways to do a French manicure?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tt3cs/easiest_ways_to_do_a_french_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>18tsxfp</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>First time trying a gradient</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqxei643v99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>18tsmla</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>New Year Nails🎆</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zn4lnysts99c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>18tsf41</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Nail Progress!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tsf41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>18tsa7j</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Recommend me a creme pastel peachy pink like this gel mani I got once, please?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enucoxj7q99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>18trms8</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>NYE skittle</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18trms8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>18trfdt</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Something simple for the holidays! 🎅❄️</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18trfdt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>18tr7af</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Venetian Sky</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tr7af</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>18tr2a2</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Subtle sunset on my nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tr2a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>18tqst0</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>How to clean under my fingernails with very short nails? Besides brushes and picking</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5qpw4gme99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>18tqb6x</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>My 2023 Fave✨</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dz3agpeua99c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>18tpim8</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Mooncat Sabertooth</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tpim8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>18tpg9t</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Cirque Colors Chiffon Dupe</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tpg9t/cirque_colors_chiffon_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>18tp8kd</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Cosmetics by Lisa - Magnetics (Velvet)</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6thkmfwb299c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>18tp1ph</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Difficult adhesion on flatter nails</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tp1ph/difficult_adhesion_on_flatter_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>18tov61</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Where do you draw the line at polishes being too similar?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tov61/where_do_you_draw_the_line_at_polishes_being_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>18topzw</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>got inspired by this sub :)</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8likdu4y89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>18toi10</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Help me decide which color</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18toi10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>18to0qu</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Millennia to ring in the new year</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dna2ncv6s89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>18tn1fm</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>I've read that Repair Mode doesn't aways help, but has anyone had it make peeling worse?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qolvngi8j89c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>18tmq93</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Something different for me</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tmq93</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>18tlpqw</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Mooncat - Mercury’s Tears</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tlpqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>18tjzub</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>I may have broken a nail but trying to make the best of it ✨</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tjzub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>18tiz31</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Which is safer to diy at home, gel nails, acrylic nails, or dip nails?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18tiz31/which_is_safer_to_diy_at_home_gel_nails_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>18u8zf9</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Obsessed with this press on nail set i did! I Love bows ✨*beginner nail artist*</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u8zf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>18u8jls</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>My painted toenails 😍♥️</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5ofcwbi5hd9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>18u8a18</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Gilded nails - chichinails Canada Ontario 🔆⚜️🔱〽️</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udxattiged9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>18u7uj2</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>I've been feeling very 2011 Tumblr vibes lately, and I'm gonna lean into it</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0o9p7c7ad9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>18u766y</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Nail set I did on a client yesterday :)</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u766y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>18u5hni</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>First time using blooming gel 💓</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm9bll8qnc9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>18u18r0</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Ginger Soul by Moxie Nail Varnish</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18u18r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>18tx9mx</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>January Blue</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tchzrs2gsa9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>18tx7ci</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>New Year’s Cows. Tech liked the idea so much he snapped a pic for Insta 😍</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h2r9acxra9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>18tt2up</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>My new year nails.</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tt2up</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>18tqig8</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>🐶🐕🐾</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18tqig8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>18tl7vx</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>My New Years set</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osgqi2qd089c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>18tisap</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>A grinchmas set I did freehand as a beginner nail tech</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dodumlj1879c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec 31 08:07:17 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_31.xlsx
+++ b/data/2023_12_31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1076"/>
+  <dimension ref="A1:C1248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18725,6 +18725,2930 @@
         </is>
       </c>
     </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>18v2tlg</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>What nail shape would suit me?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj32hi2c6l9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>18v2jje</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>[Nail health] is it necessary to take a break from polish?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18v2jje/nail_health_is_it_necessary_to_take_a_break_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>18v1mk1</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>NYE cosplay party nails</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18v1mk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>18v0v8t</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>New Year and birthday nails</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7dclgywkk9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>18v0afg</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>New set for the new year!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tz7c37t7fk9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>18uwm76</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>How to I make my apexes better??</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uwm76</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>18v08tx</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Starry cat eye!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pu9j5osek9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>18uuhac</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>How do I make my nails less flimsy?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18uuhac/how_do_i_make_my_nails_less_flimsy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>18uufyb</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>How do you get dip powder to go on smooth?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18uufyb/how_do_you_get_dip_powder_to_go_on_smooth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>18uufgk</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Not sure how to phrase this, but how can make the top part of my nails hold on better?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t0vwxh0zi9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>18uyz0t</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love how my nails came out </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f4e5586j2k9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>18uyvng</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Was feeling pastel yellow with chrome 🌞</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uyvng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>18uynzg</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>From a habitual nail bitter for years… to finding a fix with Gel💅</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uynzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>18uymyv</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Are these bad enough to get redone tomorrow?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uymyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>18uyk8n</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Trying so hard to DIY gel</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uyk8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>18uyeie</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>NYE nails</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sugwf47xj9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>18uyde0</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Black and white classic design</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uyde0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>18uybbn</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Blingy NYE nails!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2i3zajcwj9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>18uyabc</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Blue French for the new year ✨</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgf7ywm3wj9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>18uy9qm</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>In love with blue chrome powder over dark purple</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ukuw4tuxvj9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>18uxvkl</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>First time trying French tips! Any pointers?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pv2id8csj9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>18ux87q</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Nails of 2024</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ux87q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>18uwr3a</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Orly site prices vs Amazon prices?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcw6gzjdij9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>18uvgxv</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>First post!!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uvgxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>18uvcr5</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uvcr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>18uv2s4</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>New Year’s Nails 💅 🎇</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uv2s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>18uv22v</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Two month progress</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd4dpnc34j9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>18uuwes</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Obsessed with this color!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uuwes</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>18uustp</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Is this what almond nails are supposed to look like around the area where the nail joins the skin? Is it supposed to be this steeply angled. I asked for round tips and was given this instead and I’m so upset. 😞</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uustp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>18uuq8a</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>I see your holiday nails and give you my Southern Hemisphere holiday nails.</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uuq8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>18uuj2m</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>a little life in my nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjynbgyfzi9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>18utwq1</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>How’d I do with my new years nails ?💅🏾</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18utwq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>18utpap</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>First mani after baby</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzc69n99ti9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>18ut8fr</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbsg80uipi9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>18ut1j5</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>I’ve been into a lot of the japanese and chinese magnetic/abstract art ❤️</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1tcec580oi9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>18uswk8</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>January dip nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uswk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>18usqad</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>I don’t get to do Frenchies often, but my birthday is coming up and wanted to feel pretty 🩷</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8n6z7lsmli9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>18uso23</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>my version of new years nails :)</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rl170x4li9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>18uscxn</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Tried chrome powder for the first time, turned out way better than I expected!</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uscxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>18usb39</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Happy New Year!</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18usb39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>18uqcl0</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Gel overlay question</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18uqcl0/gel_overlay_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>18uqbsv</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Ocean inspiration🌊</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uqbsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>18urrxl</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Ringing in the new year with funny bunny 🎆</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs7wwlebei9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>18urg9k</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>New Year Nails - CC Welcome</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11xm3jcwbi9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>18ur6fk</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Fresh set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bm22zx0u9i9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>18ur4vu</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Grey and Orange, love them, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7s3wytti9i9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>18uqz16</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Matching my motorcycle</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ly6if0c8i9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>18uqxd8</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Redo successful</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uqxd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>18uqlqu</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Nails for New Years</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uqlqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>18uq9v7</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Got some nails done for my brother's wedding!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56iahiet2i9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>18uq00i</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>celestial robin’s egg 🪺</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdg7c7qm0i9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>18upymw</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>First time posting…a little nervous!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18upymw/first_time_postinga_little_nervous/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>18uprkd</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>New year nails</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uprkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>18uprex</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Tried gold chrome today</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gyj5bhryh9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>18upgni</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>New Years Nails</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dkd8e1kwh9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>18up69i</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Last set of the year 🍒</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18up69i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>18up3p9</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>My ethereal nails</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of08siqoth9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>18up0x3</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>what do we think? did these myself last night.</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drkilrl3th9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>18uoiks</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Hey, how can I get rid of these white things underneath my nails? It's soft gel with extension.</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uoiks</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>18uodw3</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nij9ixi5oh9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>18uo4eg</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>🍸 🫒</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hewowgc3mh9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>18unq17</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New Year's nails! The numbers were a b**** to do but I'm so happy with how they came out ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18unq17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>18unjlk</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Doing acrylics sugaring for the first time. Can I still use a UV LED soak off top coat?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18unjlk/doing_acrylics_sugaring_for_the_first_time_can_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>18unghn</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>show me your best nails of the year!!</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18unghn/show_me_your_best_nails_of_the_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>18uhzb8</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>is there supposed to be this foamy stuff all over my finger when I use nail glue? this is my first time doing something like this help O_O</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2beej9u9g9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>18ubb9w</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Where to find nail inspo?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ubb9w/where_to_find_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>18un6u2</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>New year, new nails</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18un6u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>18um8ft</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Mine and my mums nails</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w47y9v8m7h9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>18ulvfu</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>First gel set in 2 years!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ulvfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>18ulrso</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Ombre powder nails</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4yxzfu14h9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>18uljhm</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ifu6u50a2h9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>18ulgfj</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>First time getting my nails done :) thoughts?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ulgfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>18ulc3w</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Yes or no?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd92m98p0h9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>18ul2kp</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Starry starry night</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0la1xo1kyg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>18ukz0t</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Last design of the year 💫🎬</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ukz0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>18ukqmz</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>My Christmas set 🎄🎁 ngl I kinda hated it 😅😂</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ukqmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>18ukky6</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Bye bye nails</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vobxdhqug9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>18ukhu9</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Definitely one of my favorite designs I’ve gotten</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt9qr382ug9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>18uka89</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>New Year’s nails! Found a new nail tech and she brought my glitter vision to life✨</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uka89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>18uka37</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Yay my nails don’t look rubbish</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vsircjcsg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>18uk6ps</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Little sparkle for the new year! 💎</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d36wtedmrg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>18ujcew</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Question about the Kupa Manipro Passport E-File</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18ujcew/question_about_the_kupa_manipro_passport_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>18uj5q4</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Birthday Futuristic Nails</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5vwjr5kjg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>18uiwa8</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>A Fallen Soldier 😭</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a1ji9mehg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>18uiow7</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>New year, new nails</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uiow7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>18uil45</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Red nails are Lana nails</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8y9mpkxeg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>18uij6j</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Long lasting nails</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18uij6j/long_lasting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>18ui0e8</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Love my new milky white nails 😍</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oc5mdf24ag9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>18uhyxf</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>New Year's Nails!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7d7o4yq9g9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>18uhsp1</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Just a super sparkly set for nee years 🕰️✨</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uhsp1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>18uhrua</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Silver (chrome) nails for New Year!!🎊🎈🎆</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tglgoi138g9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>18uhbvg</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Solar changing polygel nails ✨</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kdotiu5d4g9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>18ugex4</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Prepare your eyeballs!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ugex4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>18ugeld</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>A bronze moment ✨</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ugeld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>18ugbdi</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>New Year Nails. (+ How can I get the glitter of my skin?)</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ugbdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>18ufqth</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p7xd5lxpf9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>18ufprs</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>New years nails</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vef9ihynpf9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>18ufoch</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Nails for New Year</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ufoch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>18ufmq9</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>I always get distracted by my nail polish when I work out</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izqk7f6vof9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>18ufiza</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dch8ff4unf9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>18v19m0</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>New Years Mani</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18v19m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>18v15tl</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>New year nails!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unwo4ohunk9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>18uzwgj</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Does anyone have an ingredient list for the colored Sally Hansen Hard as Nails polishes?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18uzwgj/does_anyone_have_an_ingredient_list_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>18uzqqy</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>I love this subreddit so much. We really are just sum crows who gravitate towards anything shiny or sparkly that we can express ourselves with— that's so beautiful of us</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18uzqqy/i_love_this_subreddit_so_much_we_really_are_just/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>18uzip6</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Natty Nail After Dip</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uzip6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>18uzigj</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>NYE mani!!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57qn75hq7k9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>18uywki</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>How is the ILNP customer service? Specifics in post</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18uywki/how_is_the_ilnp_customer_service_specifics_in_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>18uxo3i</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Last mani of the year</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uxo3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>18ux9ii</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>NYE Mani!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ux9ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>18ux17f</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Polish you can't import into the US?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18ux17f/polish_you_cant_import_into_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>18uwuis</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Swatches of a neutral pink purple shimmer kinda girlie</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uwuis</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>18uwbwu</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>my favorite nude nail polish!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs6jvcvpej9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>18uvz6a</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>A post from this group inspiring me in 2024…</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ndzr52zobj9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>18uv86k</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Deep Space</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uv86k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>18uv28p</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Tiny polish!! 🥹</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8xibyo44j9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>18uuzo1</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>New Year’s wraps! Black &amp; gold glitter chevron &amp; stripes ✨</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtcd7v1j3j9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>18uup1d</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>My entire polish collection sorted by brand</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uup1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>18uugqv</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Back with another thermal obsession</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uugqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>18uug7h</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>branded vs diy jellies?</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18uug7h/branded_vs_diy_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>18uuet2</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Covid swatches complete</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uuet2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>18uu89v</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Blue laser beams 🩵</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdmzn5cexi9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>18utd5k</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>I have so many goddamn purples</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18utd5k/i_have_so_many_goddamn_purples/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>18usg4f</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Tried chrome powder for the first time, turned out way better than I expected!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18usg4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>18uqx5l</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Essie- sugar daddy</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/372hprww7i9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>18urdaz</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Glass jellyfish gang 🪼</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18urdaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>18uq1ap</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>🥂 You won't remember all my champagne problems 🥂</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uq1ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>18upuqj</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>My 2023 Nails 💕</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18upuqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>18upruo</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Mermaid-y NYE skittle claws</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18upruo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>18upggx</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Light blue cat eye</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzm39naiwh9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>18updbj</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Advice for stars needed</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18updbj/advice_for_stars_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>18upcsv</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>OPI - I'm Really An Actress 👠</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18upcsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>18upcsf</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>💅🏻favorite manis of 2023💅🏻</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18upcsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>18up098</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Oxblood</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18up098</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>18uosbf</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Acrylic Nail Set For Graduating Nail School!</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uosbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>18uobr9</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Happy New Year! ✨</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mswpfh2onh9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>18unqmb</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Somewhat different starry sky: Penelope Luz - Movie Night</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18unqmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>18unpal</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fairy Dust vs Truth is Painful </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/abgwso4wih9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>18un68r</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>New years shimmer!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18un68r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>18umyve</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>🧡🌴Miami Vaporwave🌴💜</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18umyve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>18umdqs</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>how to secure charms on natural nails + regular polish?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18umdqs/how_to_secure_charms_on_natural_nails_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>18umdji</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Mooncat Bootlegger</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18umdji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>18um3hw</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>New Years Nails!</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5xfidzg6h9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>18um0d4</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Got my first mooncat for my birthday!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18um0d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>18ulysg</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>accepting thoughts and prayers for 2024</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42siglqh5h9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>18ultmg</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>First ILNP Pick Up</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6pnnoof4h9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>18ult2m</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Couldn't decide on which sparkly polish to wear for New Year's so I decided to wear them all</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ult2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>18ul6fs</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Tried my hand at nail stamping! My second attempt</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaiwlaxezg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>18uktj8</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Haunted Melody</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uktj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>18ukr4p</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>{PR} Don’t Touch the Calico Bush!</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77tatds2wg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>18uklbs</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>nye mani!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6d98f21tug9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>18uivpl</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>'Pop Colour' Topper</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18uivpl/pop_colour_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>18uikhm</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Coronation 2023</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p2zhohseg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>18uijp2</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>New Year's nails and first gradient</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/i77giKp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>18uiiqc</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>still my favorite “nude but make it sparkly” ✨</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uiiqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>18uhzg5</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>My right thumb nail has ALWAYS done this. Anything I can do? I use a glass nail file.</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmj04bev9g9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>18uhdvj</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Throwback to my natural nails! Any recommendations on polishes you think would be flattering?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3itahn3v4g9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>18ugo11</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Full glitter is a must for new years!</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ugo11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>18ug1f3</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>ILNP Carrie 🩸</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rp2ylkqsf9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>18ufxik</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Le Mini Macaron mix: 2 drops Café Crème and 1 drop Sugar Crush</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f0mzvx0orf9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>18ufncv</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Like a decorated Christmas tree </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/151co771pf9c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>18uflqr</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>I always get distracted by my nail polish when I work out</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvtsia2lof9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>18uez9o</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>jump scare! my natural nails, longest and strongest they’ve ever been 🩶</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uez9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>18uerl6</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Best Jellies? Preferably with no effects but a subtle scattered holo or other subtle effects are okay</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18uerl6/best_jellies_preferably_with_no_effects_but_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>18ue374</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>First time trying a glitter gradient! ❄️</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ue374</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>18udoa7</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Order arrived early! Can't wait to try them [Clionadh Cosmetics]</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18udoa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>18uy284</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18uy284</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>18uvvfi</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>🎆 🎇 New Year Set 🎇🎆</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lehx11taj9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>18uvdqa</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Gel nails 🎇🎆</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/474wwe3p6j9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>18upfpl</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Light blue cat eye on natural nails</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vewpdc1cwh9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>18unm30</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Better quality photo of my gilded nails chichi nails in ontario 🔆🔱⚜️〽️</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht248vv6ih9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>18ukqyf</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>New S-Gel Set</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhs0ilbvvg9c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>18ujqvg</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>New Year's nails ❣️🥳</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18ujqvg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>